<commit_message>
Finished general route and added switches
</commit_message>
<xml_diff>
--- a/levels.xlsx
+++ b/levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\z git\zbols-secretsanta2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4FC103-3A19-40B4-86D2-9E18E948D2EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F19FAC-8B7A-4BB6-92D7-2C7BDEE330E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4F033241-C44B-43F5-97F3-F0CACB9C553E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="45">
   <si>
     <t>Wall</t>
   </si>
@@ -144,6 +143,33 @@
   <si>
     <t xml:space="preserve"> 1F</t>
   </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Switch Gate</t>
+  </si>
+  <si>
+    <t>Inv. Sw. Gate</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>\1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +216,52 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="155">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color rgb="FFC71111"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFF8AEAE"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFC71111"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -372,10 +443,1931 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color rgb="FFC71111"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFF8AEAE"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFC71111"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color rgb="FFC71111"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFF8AEAE"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFC71111"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color rgb="FFC71111"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFF8AEAE"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFC71111"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC71111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC71111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC71111"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF722FB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color rgb="FFC00000"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="9" tint="0.80001220740379042"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="7" tint="0.40000610370189521"/>
+          </stop>
+          <stop position="1">
+            <color theme="5" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF8AEAE"/>
+      <color rgb="FFC71111"/>
       <color rgb="FF722FB5"/>
     </mruColors>
   </colors>
@@ -691,7 +2683,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE20" sqref="AE20"/>
+      <selection pane="topRight" activeCell="AH10" sqref="AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,6 +2935,9 @@
       <c r="BC2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BN2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="BO2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1017,6 +3012,9 @@
       <c r="AP3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BB3" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="BC3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1103,6 +3101,12 @@
       <c r="AP4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AQ4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BC4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1174,6 +3178,12 @@
       <c r="AP5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="AQ5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BC5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1257,6 +3267,12 @@
       <c r="AP6" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AQ6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="BC6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1365,13 +3381,13 @@
         <v>2</v>
       </c>
       <c r="AX7" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="AY7" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="AZ7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA7" s="1" t="s">
         <v>1</v>
@@ -1531,6 +3547,27 @@
       <c r="AR8" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AS8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA8" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="BB8" s="1">
         <v>9</v>
       </c>
@@ -1662,6 +3699,15 @@
       <c r="AR9" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AS9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="BB9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1715,8 +3761,26 @@
       <c r="AR10" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="AS10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="BB10" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="BK10" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="BO10" s="1" t="s">
         <v>1</v>
@@ -1771,6 +3835,9 @@
       <c r="AR11" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BA11" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="BB11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1824,11 +3891,20 @@
       <c r="AR12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="AU12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY12" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="BB12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="BK12" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="BO12" s="1" t="s">
         <v>1</v>
@@ -1871,8 +3947,17 @@
       <c r="AR13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BA13" s="1" t="s">
+      <c r="AU13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX13" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="AY13" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="BB13" s="1" t="s">
         <v>1</v>
@@ -1888,6 +3973,12 @@
       </c>
     </row>
     <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1924,11 +4015,11 @@
       <c r="N14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="1" t="s">
-        <v>1</v>
+      <c r="O14" s="1">
+        <v>13</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>1</v>
@@ -2003,11 +4094,11 @@
         <v>10</v>
       </c>
       <c r="AT14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AU14" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="AV14" s="1" t="s">
         <v>1</v>
       </c>
@@ -2029,8 +4120,8 @@
       <c r="BB14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BC14" s="1" t="s">
-        <v>1</v>
+      <c r="BC14" s="1">
+        <v>20</v>
       </c>
       <c r="BD14" s="1" t="s">
         <v>1</v>
@@ -2097,6 +4188,12 @@
       </c>
     </row>
     <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
@@ -2171,6 +4268,12 @@
       </c>
     </row>
     <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
@@ -2327,8 +4430,8 @@
       </c>
     </row>
     <row r="22" spans="3:69" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
-        <v>1</v>
+      <c r="C22" s="1">
+        <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -2360,8 +4463,8 @@
       <c r="M22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>1</v>
+      <c r="N22" s="1">
+        <v>14</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>1</v>
@@ -2393,8 +4496,8 @@
       <c r="X22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Y22" s="1" t="s">
-        <v>1</v>
+      <c r="Y22" s="1">
+        <v>16</v>
       </c>
       <c r="Z22" s="1" t="s">
         <v>1</v>
@@ -2426,8 +4529,8 @@
       <c r="AI22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AJ22" s="1" t="s">
-        <v>1</v>
+      <c r="AJ22" s="1">
+        <v>17</v>
       </c>
       <c r="AK22" s="1" t="s">
         <v>1</v>
@@ -2459,8 +4562,8 @@
       <c r="AT22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AU22" s="1" t="s">
-        <v>1</v>
+      <c r="AU22" s="1">
+        <v>18</v>
       </c>
       <c r="AV22" s="1" t="s">
         <v>1</v>
@@ -2492,8 +4595,8 @@
       <c r="BE22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BF22" s="1" t="s">
-        <v>1</v>
+      <c r="BF22" s="1">
+        <v>19</v>
       </c>
       <c r="BG22" s="1" t="s">
         <v>1</v>
@@ -2872,44 +4975,53 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="31" priority="11">
       <formula>AND(LEFT(A1)="G",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="30" priority="12">
       <formula>AND(LEFT(A1)="K",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="26" priority="16">
       <formula>AND(NOT(ISBLANK(A1)),OR(LEFT(A1)=" ",NOT(ISERROR(INT(A1)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="10">
       <formula>AND(LEFT(A1)="F",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="24" priority="9">
       <formula>AND(LEFT(A1)="E",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
       <formula>"_"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"*"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="3">
+      <formula>AND(LEFT(A1)="\",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="2">
+      <formula>AND(LEFT(A1)="S",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="1">
+      <formula>AND(LEFT(A1)="Z",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Placed Doors and other pathways
</commit_message>
<xml_diff>
--- a/levels.xlsx
+++ b/levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\z git\zbols-secretsanta2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F19FAC-8B7A-4BB6-92D7-2C7BDEE330E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C28B330-20ED-4292-96FE-C07639AF8F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4F033241-C44B-43F5-97F3-F0CACB9C553E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="49">
   <si>
     <t>Wall</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Z1</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Crowbar</t>
+  </si>
+  <si>
+    <t>Step=ladder</t>
+  </si>
+  <si>
+    <t>^</t>
   </si>
 </sst>
 </file>
@@ -216,7 +228,24 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="155">
+  <dxfs count="102">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="7"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -445,6 +474,67 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="270">
+          <stop position="0">
+            <color theme="9" tint="0.59999389629810485"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="7"/>
+          </stop>
+          <stop position="1">
+            <color theme="9"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color rgb="FFC71111"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFF8AEAE"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFC71111"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8AEAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -459,33 +549,6 @@
             <color theme="0"/>
           </stop>
         </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color rgb="FFC71111"/>
-          </stop>
-          <stop position="0.5">
-            <color rgb="FFF8AEAE"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFC71111"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8AEAE"/>
-        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -671,6 +734,23 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0" tint="-0.34900967436750391"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.25098422193060094"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
         <color theme="0"/>
@@ -897,9 +977,26 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="1"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="-0.49803155613879818"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
-        <color theme="1"/>
+        <color theme="0"/>
       </font>
       <fill>
         <gradientFill degree="45">
@@ -1123,12 +1220,39 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC71111"/>
-        </patternFill>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="9" tint="-0.49803155613879818"/>
+          </stop>
+          <stop position="1">
+            <color theme="1"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color rgb="FFC71111"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFF8AEAE"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFC71111"/>
+          </stop>
+        </gradientFill>
       </fill>
     </dxf>
     <dxf>
@@ -1339,12 +1463,22 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC71111"/>
-        </patternFill>
+        <b val="0"/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color rgb="FFC71111"/>
+          </stop>
+          <stop position="0.5">
+            <color rgb="FFF8AEAE"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFC71111"/>
+          </stop>
+        </gradientFill>
       </fill>
     </dxf>
     <dxf>
@@ -1553,821 +1687,12 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC71111"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8AEAE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="0.5">
-            <color rgb="FFC00000"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF722FB5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color rgb="FFC00000"/>
-          </stop>
-          <stop position="1">
-            <color theme="9" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="9" tint="0.80001220740379042"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path">
-          <stop position="0">
-            <color theme="9" tint="0.59999389629810485"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color theme="7" tint="0.40000610370189521"/>
-          </stop>
-          <stop position="1">
-            <color theme="5" tint="0.40000610370189521"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8AEAE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="0.5">
-            <color rgb="FFC00000"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF722FB5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color rgb="FFC00000"/>
-          </stop>
-          <stop position="1">
-            <color theme="9" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="9" tint="0.80001220740379042"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path">
-          <stop position="0">
-            <color theme="9" tint="0.59999389629810485"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color theme="7" tint="0.40000610370189521"/>
-          </stop>
-          <stop position="1">
-            <color theme="5" tint="0.40000610370189521"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8AEAE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="0.5">
-            <color rgb="FFC00000"/>
-          </stop>
-          <stop position="1">
-            <color theme="0"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF722FB5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color rgb="FFC00000"/>
-          </stop>
-          <stop position="1">
-            <color theme="9" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="9" tint="0.80001220740379042"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path">
-          <stop position="0">
-            <color theme="9" tint="0.59999389629810485"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color theme="7" tint="0.40000610370189521"/>
-          </stop>
-          <stop position="1">
-            <color theme="5" tint="0.40000610370189521"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF722FB5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color rgb="FFC00000"/>
-          </stop>
-          <stop position="1">
-            <color theme="9" tint="-0.25098422193060094"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="9" tint="0.80001220740379042"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <gradientFill type="path">
-          <stop position="0">
-            <color theme="9" tint="0.59999389629810485"/>
-          </stop>
-          <stop position="1">
-            <color theme="9"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <gradientFill degree="45">
-          <stop position="0">
-            <color theme="7" tint="0.40000610370189521"/>
-          </stop>
-          <stop position="1">
-            <color theme="5" tint="0.40000610370189521"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC71111"/>
       <color rgb="FFF8AEAE"/>
-      <color rgb="FFC71111"/>
       <color rgb="FF722FB5"/>
     </mruColors>
   </colors>
@@ -2679,11 +2004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065F18A9-66B3-4988-8845-BB8707C2A249}">
-  <dimension ref="A1:CI29"/>
+  <dimension ref="A1:CJ29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH10" sqref="AH10"/>
+      <selection pane="topRight" activeCell="AT20" sqref="AT20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="CA1" s="1" t="s">
         <v>1</v>
@@ -2942,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="BP2" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="BQ2" s="1" t="s">
         <v>1</v>
@@ -3117,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="BY4" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="CI4" s="1" t="s">
         <v>1</v>
@@ -3408,7 +2733,7 @@
         <v>1</v>
       </c>
       <c r="CA7" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="CB7" s="1" t="s">
         <v>1</v>
@@ -3417,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="CD7" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="CE7" s="1" t="s">
         <v>1</v>
@@ -3611,7 +2936,7 @@
         <v>1</v>
       </c>
       <c r="BP8" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="BQ8" s="1" t="s">
         <v>1</v>
@@ -3626,7 +2951,7 @@
         <v>1</v>
       </c>
       <c r="BU8" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BV8" s="1" t="s">
         <v>1</v>
@@ -3649,7 +2974,7 @@
     </row>
     <row r="9" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -3779,6 +3104,9 @@
       <c r="BB10" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BC10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="BK10" s="1" t="s">
         <v>32</v>
       </c>
@@ -3786,7 +3114,7 @@
         <v>1</v>
       </c>
       <c r="BZ10" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="CH10" s="1" t="s">
         <v>1</v>
@@ -3842,7 +3170,7 @@
         <v>1</v>
       </c>
       <c r="BO11" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="BZ11" s="1" t="s">
         <v>1</v>
@@ -3906,6 +3234,9 @@
       <c r="BB12" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="BN12" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="BO12" s="1" t="s">
         <v>1</v>
       </c>
@@ -3979,11 +3310,11 @@
       <c r="B14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>1</v>
+      <c r="C14" s="1">
+        <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>1</v>
@@ -4121,10 +3452,10 @@
         <v>1</v>
       </c>
       <c r="BC14" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="BD14" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="BE14" s="1" t="s">
         <v>1</v>
@@ -4163,7 +3494,7 @@
         <v>1</v>
       </c>
       <c r="CA14" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="CB14" s="1" t="s">
         <v>1</v>
@@ -4175,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="CE14" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="CF14" s="1" t="s">
         <v>1</v>
@@ -4184,6 +3515,9 @@
         <v>1</v>
       </c>
       <c r="CH14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI14" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4233,11 +3567,11 @@
       <c r="BO15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BP15" s="1" t="s">
-        <v>1</v>
+      <c r="BP15" s="1">
+        <v>22</v>
       </c>
       <c r="BQ15" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="BR15" s="1" t="s">
         <v>1</v>
@@ -4264,6 +3598,9 @@
         <v>1</v>
       </c>
       <c r="BZ15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4281,7 +3618,7 @@
         <v>1</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AH16" s="1" t="s">
         <v>1</v>
@@ -4295,8 +3632,20 @@
       <c r="BP16" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI16" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
@@ -4307,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="AH17" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AS17" s="1" t="s">
         <v>1</v>
@@ -4316,15 +3665,27 @@
         <v>1</v>
       </c>
       <c r="BP17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BZ17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI17" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="Y18" s="1" t="s">
         <v>1</v>
@@ -4341,8 +3702,14 @@
       <c r="BP18" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI18" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
@@ -4356,7 +3723,7 @@
         <v>1</v>
       </c>
       <c r="AS19" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="BC19" s="1" t="s">
         <v>1</v>
@@ -4364,8 +3731,14 @@
       <c r="BP19" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI19" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
@@ -4387,8 +3760,14 @@
       <c r="BP20" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI20" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
@@ -4428,19 +3807,25 @@
       <c r="BP21" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI21" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>1</v>
@@ -4467,7 +3852,7 @@
         <v>14</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>1</v>
@@ -4497,10 +3882,10 @@
         <v>1</v>
       </c>
       <c r="Y22" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>1</v>
@@ -4530,10 +3915,10 @@
         <v>1</v>
       </c>
       <c r="AJ22" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="AL22" s="1" t="s">
         <v>1</v>
@@ -4563,10 +3948,10 @@
         <v>1</v>
       </c>
       <c r="AU22" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AV22" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="AW22" s="1" t="s">
         <v>1</v>
@@ -4596,10 +3981,10 @@
         <v>1</v>
       </c>
       <c r="BF22" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BG22" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="BH22" s="1" t="s">
         <v>1</v>
@@ -4608,7 +3993,7 @@
         <v>1</v>
       </c>
       <c r="BJ22" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="BK22" s="1" t="s">
         <v>1</v>
@@ -4628,11 +4013,68 @@
       <c r="BP22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BQ22" s="1" t="s">
+      <c r="BQ22" s="1">
+        <v>23</v>
+      </c>
+      <c r="BR22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BS22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BU22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BV22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BX22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BY22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BZ22" s="1">
+        <v>24</v>
+      </c>
+      <c r="CA22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="CB22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CC22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CD22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CE22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CF22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CG22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CH22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ22" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
@@ -4654,8 +4096,14 @@
       <c r="BQ23" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ23" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
@@ -4669,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="AU24" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="BF24" s="1" t="s">
         <v>1</v>
@@ -4677,8 +4125,14 @@
       <c r="BQ24" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ24" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
@@ -4689,19 +4143,25 @@
         <v>1</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AU25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="BF25" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="BQ25" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="CJ25" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="26" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>1</v>
       </c>
@@ -4709,7 +4169,7 @@
         <v>1</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AJ26" s="1" t="s">
         <v>1</v>
@@ -4723,8 +4183,14 @@
       <c r="BQ26" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ26" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="27" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
@@ -4746,8 +4212,14 @@
       <c r="BQ27" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BZ27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ27" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>1</v>
       </c>
@@ -4769,8 +4241,38 @@
       <c r="BQ28" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="BR28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BU28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BV28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BX28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BY28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BZ28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ28" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:88" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>1</v>
       </c>
@@ -4970,58 +4472,97 @@
         <v>1</v>
       </c>
       <c r="BQ29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BZ29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CA29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CB29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CC29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CD29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CE29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CF29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CG29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CH29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CJ29" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="31" priority="11">
+    <cfRule type="expression" dxfId="34" priority="13">
       <formula>AND(LEFT(A1)="G",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="12">
+    <cfRule type="expression" dxfId="33" priority="14">
       <formula>AND(LEFT(A1)="K",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="15" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="16" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="17" operator="equal">
       <formula>"W"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="16">
+    <cfRule type="expression" dxfId="29" priority="18">
       <formula>AND(NOT(ISBLANK(A1)),OR(LEFT(A1)=" ",NOT(ISERROR(INT(A1)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="10">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>AND(LEFT(A1)="F",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="9">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>AND(LEFT(A1)="E",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
       <formula>"L"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"V"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
       <formula>"_"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"*"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>AND(LEFT(A1)="\",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>AND(LEFT(A1)="S",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>AND(LEFT(A1)="Z",OR(NOT(ISERROR(VALUE(RIGHT(A1,LEN(A1)-1)))),LEN(A1)=1))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+      <formula>"%"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"^"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
75% of Levels done
</commit_message>
<xml_diff>
--- a/levels.xlsx
+++ b/levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Zak\Documents\GitHub\zbols-secretsanta2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BA15BF-1DBD-4B1B-9315-13F3E9A48579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F512CED1-8530-4D58-9535-4307834CB2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4F033241-C44B-43F5-97F3-F0CACB9C553E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="269">
   <si>
     <t>Wall</t>
   </si>
@@ -1599,11 +1599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065F18A9-66B3-4988-8845-BB8707C2A249}">
-  <dimension ref="A1:CK37"/>
+  <dimension ref="A1:CK39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CD10" sqref="CD10"/>
+      <selection pane="topRight" activeCell="BI18" sqref="BI18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,12 +1679,6 @@
       <c r="AX1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="BA1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1890,15 +1884,17 @@
       </c>
       <c r="AW2" s="3"/>
       <c r="AX2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="BA2" s="3"/>
+      <c r="BA2" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="BB2" s="3" t="s">
         <v>2</v>
       </c>
@@ -7234,6 +7230,9 @@
       </c>
     </row>
     <row r="30" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="S30" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AD30" s="1" t="s">
         <v>146</v>
       </c>
@@ -7254,6 +7253,9 @@
       </c>
     </row>
     <row r="31" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="S31" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AD31" s="1" t="s">
         <v>1</v>
       </c>
@@ -7274,6 +7276,9 @@
       </c>
     </row>
     <row r="32" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="S32" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AG32" s="1" t="s">
         <v>1</v>
       </c>
@@ -7293,7 +7298,10 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="21:70" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:70" x14ac:dyDescent="0.25">
+      <c r="S33" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="U33" s="1" t="s">
         <v>1</v>
       </c>
@@ -7337,7 +7345,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="21:70" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:70" x14ac:dyDescent="0.25">
+      <c r="S34" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="V34" s="1" t="s">
         <v>1</v>
       </c>
@@ -7402,7 +7413,25 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="21:70" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:70" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="U35" s="1" t="s">
         <v>1</v>
       </c>
@@ -7437,7 +7466,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="21:70" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:70" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AQ36" s="1" t="s">
         <v>115</v>
       </c>
@@ -7445,9 +7495,130 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="21:70" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:70" x14ac:dyDescent="0.25">
+      <c r="F37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="BG37" s="1" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="4:70" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:70" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished basic structure of all Levels
</commit_message>
<xml_diff>
--- a/levels.xlsx
+++ b/levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Zak\Documents\GitHub\zbols-secretsanta2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F512CED1-8530-4D58-9535-4307834CB2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17133A0D-A286-4F6E-B8E0-57D277DD96EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4F033241-C44B-43F5-97F3-F0CACB9C553E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="269">
   <si>
     <t>Wall</t>
   </si>
@@ -841,7 +841,7 @@
     <t>X3</t>
   </si>
   <si>
-    <t>[[ 1`</t>
+    <t>F-3</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BI18" sqref="BI18"/>
+      <selection pane="topRight" activeCell="BT25" sqref="BT25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4795,7 +4795,9 @@
       <c r="AK17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AL17" s="4"/>
+      <c r="AL17" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="AM17" s="4"/>
       <c r="AN17" s="4"/>
       <c r="AO17" s="4"/>
@@ -5142,7 +5144,9 @@
         <v>8</v>
       </c>
       <c r="AR19" s="4"/>
-      <c r="AS19" s="4"/>
+      <c r="AS19" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="AT19" s="4" t="s">
         <v>145</v>
       </c>
@@ -5182,7 +5186,9 @@
         <v>2</v>
       </c>
       <c r="BH19" s="6"/>
-      <c r="BI19" s="6"/>
+      <c r="BI19" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="BJ19" s="6" t="s">
         <v>88</v>
       </c>
@@ -5395,7 +5401,9 @@
       <c r="BK20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="BL20" s="6"/>
+      <c r="BL20" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="BM20" s="6"/>
       <c r="BN20" s="6" t="s">
         <v>95</v>
@@ -6202,7 +6210,9 @@
       <c r="AO24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AP24" s="6"/>
+      <c r="AP24" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="AQ24" s="6"/>
       <c r="AR24" s="6" t="s">
         <v>2</v>
@@ -6408,9 +6418,7 @@
       </c>
       <c r="BH25" s="6"/>
       <c r="BI25" s="6"/>
-      <c r="BJ25" s="6" t="s">
-        <v>268</v>
-      </c>
+      <c r="BJ25" s="6"/>
       <c r="BK25" s="6"/>
       <c r="BL25" s="6"/>
       <c r="BM25" s="6"/>
@@ -6529,13 +6537,13 @@
       <c r="AL26" s="6"/>
       <c r="AM26" s="6"/>
       <c r="AN26" s="6"/>
-      <c r="AO26" s="6"/>
+      <c r="AO26" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="AP26" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AQ26" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="AQ26" s="6"/>
       <c r="AR26" s="6"/>
       <c r="AS26" s="6"/>
       <c r="AT26" s="6"/>
@@ -6690,14 +6698,10 @@
       <c r="AM27" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AN27" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN27" s="6"/>
       <c r="AO27" s="6"/>
       <c r="AP27" s="6"/>
-      <c r="AQ27" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="AQ27" s="6"/>
       <c r="AR27" s="6"/>
       <c r="AS27" s="6"/>
       <c r="AT27" s="6"/>
@@ -6715,7 +6719,9 @@
         <v>88</v>
       </c>
       <c r="AZ27" s="6"/>
-      <c r="BA27" s="6"/>
+      <c r="BA27" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="BB27" s="6" t="s">
         <v>2</v>
       </c>
@@ -6765,9 +6771,7 @@
       <c r="BX27" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="BY27" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="BY27" s="6"/>
       <c r="BZ27" s="6" t="s">
         <v>90</v>
       </c>
@@ -6882,7 +6886,9 @@
       </c>
       <c r="AP28" s="6"/>
       <c r="AQ28" s="6"/>
-      <c r="AR28" s="6"/>
+      <c r="AR28" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="AS28" s="6" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
25% of Levels Adjusted
</commit_message>
<xml_diff>
--- a/levels.xlsx
+++ b/levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Zak\Documents\GitHub\zbols-secretsanta2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17133A0D-A286-4F6E-B8E0-57D277DD96EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488AABF1-EA9E-46EA-848F-B46D9044D5E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4F033241-C44B-43F5-97F3-F0CACB9C553E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="269">
   <si>
     <t>Wall</t>
   </si>
@@ -1603,7 +1603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BT25" sqref="BT25"/>
+      <selection pane="topRight" activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5939,6 +5939,9 @@
     <row r="23" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>89</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>90</v>

</xml_diff>